<commit_message>
delete some stuff and change the path for some files
</commit_message>
<xml_diff>
--- a/data/Geocoding/Alpha.xlsx
+++ b/data/Geocoding/Alpha.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zt/Desktop/2023 Spring/TA GIS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zt/Desktop/Geocoding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C02D30A-1D99-C943-9367-1BC68BC191B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4821282-ECDB-FB47-9ED7-EDA3D14CA41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="1060" windowWidth="28240" windowHeight="16940" xr2:uid="{5FE1011C-61D1-AA43-B58B-D1FE328129D1}"/>
+    <workbookView xWindow="13720" yWindow="1580" windowWidth="28240" windowHeight="16940" xr2:uid="{5FE1011C-61D1-AA43-B58B-D1FE328129D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t xml:space="preserve">Location </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -163,6 +163,26 @@
   </si>
   <si>
     <t>Greenpoint Landing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>264 North 10th Street</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>81-111 Junius Street</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ralph Avenue and Preston Court</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can not find the address, not specific</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11212-8004</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -214,10 +234,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,31 +553,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DED13BB-576E-EF40-9C26-D292C1B64F58}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -568,13 +588,13 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>40.684998</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>-73.974341999999993</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -582,13 +602,13 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>40.757088000000003</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>-73.242194999999995</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -596,13 +616,13 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>40.702025999999996</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>-73.948830000000001</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -610,13 +630,13 @@
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>40.605549000000003</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>73.985397000000006</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -624,135 +644,175 @@
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>40.676780999999998</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>-73.897591000000006</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>40.678058999999998</v>
-      </c>
-      <c r="C7">
-        <v>-73.883240000000001</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <v>40.677475000000001</v>
-      </c>
-      <c r="C8">
-        <v>-73.921486000000002</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
+        <v>40.678058999999998</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-73.883240000000001</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9">
-        <v>40.716346999999999</v>
-      </c>
-      <c r="C9">
-        <v>-73.951674999999994</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="B9" s="1">
+        <v>40.677475000000001</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-73.921486000000002</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10">
-        <v>40.688949999999998</v>
-      </c>
-      <c r="C10">
-        <v>-73.981414999999998</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="B10" s="1">
+        <v>40.703570999999997</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-73.984756000000004</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
-        <v>40.703570999999997</v>
-      </c>
-      <c r="C11">
-        <v>-73.984756000000004</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="B11" s="1">
+        <v>40.716346999999999</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-73.951674999999994</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="B12" s="1">
+        <v>40.688949999999998</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-73.981414999999998</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13">
-        <v>40.675457000000002</v>
-      </c>
-      <c r="C13">
-        <v>-73.881362999999993</v>
-      </c>
-      <c r="D13" s="2">
-        <v>11208</v>
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14">
-        <v>40.675381000000002</v>
-      </c>
-      <c r="C14">
-        <v>-73.879638999999997</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="B14" s="1">
+        <v>40.675457000000002</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-73.881362999999993</v>
+      </c>
+      <c r="D14" s="1">
+        <v>11208</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1">
+        <v>40.672759999999997</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-73.903649999999999</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1">
+        <v>40.675381000000002</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-73.879638999999997</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E17" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1">
+        <v>40.641182000000001</v>
+      </c>
+      <c r="C18" s="1">
+        <v>-73.919568999999996</v>
+      </c>
+      <c r="D18" s="1">
+        <v>11234</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E18">
+    <sortCondition ref="A3:A18"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>